<commit_message>
in progress cigna plan
</commit_message>
<xml_diff>
--- a/Input/Cigna_Global_Health/benefits.xlsx
+++ b/Input/Cigna_Global_Health/benefits.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="168">
   <si>
     <t xml:space="preserve">PlanName</t>
   </si>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t xml:space="preserve">OP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dental - Optical Benefits</t>
   </si>
   <si>
     <t xml:space="preserve">Gold</t>
@@ -531,7 +534,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -553,6 +556,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -597,7 +606,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -608,6 +617,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -623,25 +636,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AZ50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AT1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AZ17" activeCellId="0" sqref="AZ17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AS1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AZ4" activeCellId="0" sqref="AZ4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="1" style="0" width="8.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="17.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="52.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="53" style="0" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -799,7 +810,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
@@ -957,7 +968,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>85</v>
       </c>
@@ -1084,13 +1095,16 @@
       <c r="AY3" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AZ3" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>54</v>
@@ -1114,7 +1128,7 @@
         <v>57</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>57</v>
@@ -1144,7 +1158,7 @@
         <v>48</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="U4" s="1" t="s">
         <v>61</v>
@@ -1153,7 +1167,7 @@
         <v>60</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="X4" s="1" t="s">
         <v>64</v>
@@ -1168,10 +1182,10 @@
         <v>64</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AD4" s="1" t="s">
         <v>64</v>
@@ -1198,10 +1212,10 @@
         <v>70</v>
       </c>
       <c r="AL4" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AM4" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AS4" s="1" t="s">
         <v>30</v>
@@ -1209,10 +1223,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL5" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AM5" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AS5" s="1" t="s">
         <v>26</v>
@@ -1220,10 +1234,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL6" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AM6" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AS6" s="1" t="s">
         <v>24</v>
@@ -1231,267 +1245,267 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL7" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="AM7" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL8" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AM8" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL9" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AM9" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL10" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AM10" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL11" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AM11" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL12" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AM12" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL13" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AM13" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL14" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AM14" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL15" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AM15" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL16" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AM16" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL17" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AM17" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL18" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AM18" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL19" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AM19" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL20" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AM20" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL21" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AM21" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL22" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL23" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL24" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL25" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL26" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL27" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL28" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL29" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL30" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL31" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL32" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL33" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL34" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL35" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL36" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL37" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL38" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL39" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL40" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL41" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL42" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL43" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL44" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL45" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL46" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL47" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL48" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL49" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL50" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>